<commit_message>
Changed excel chart and data
</commit_message>
<xml_diff>
--- a/excel test with ploot.xlsx
+++ b/excel test with ploot.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbalc\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbalc\OneDrive\Documents\AAA git\Pre-FDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$3:$B$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$3:$C$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3:$B$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$3:$C$20</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +31,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,8 +67,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +447,446 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-284C-42C3-A358-B41AE15562F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-284C-42C3-A358-B41AE15562F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="649796352"/>
+        <c:axId val="649800288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="649796352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="649800288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="649800288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="649796352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -989,6 +1442,514 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1022,6 +1983,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>179070</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>483870</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1713940-3E85-4690-9EBA-5F712F5959CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1327,116 +2324,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB833DA6-4B90-4E8F-8262-8D80E188C77F}">
-  <dimension ref="B3:C15"/>
+  <dimension ref="B3:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C15"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8">
+      <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11">
+      <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12">
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13">
+      <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14">
+      <c r="B14" s="1">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15">
+      <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3rd change to this excel file
a bar graph added
</commit_message>
<xml_diff>
--- a/excel test with ploot.xlsx
+++ b/excel test with ploot.xlsx
@@ -846,6 +846,64 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{4FCCF166-FBE3-4B83-AB79-3381D949E1A4}" formatIdx="0">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="clusteredColumn" hidden="1" uniqueId="{B19D8C88-795B-499B-A7DD-F069504BE526}" formatIdx="2">
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{360F8145-100A-499B-9995-4647E6ABF79F}" formatIdx="1">
+          <cx:axisId val="2"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="1" uniqueId="{B655F6B5-7D76-4F82-A3EB-8C242454010A}" formatIdx="3">
+          <cx:axisId val="2"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -926,6 +984,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1950,20 +2048,528 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>179070</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>300990</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>483870</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>605790</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1990,16 +2596,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>179070</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>483870</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2022,6 +2628,84 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>544830</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>240030</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03B148CC-D3AE-486D-8556-C38D94090D9B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8469630" y="1203960"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2326,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB833DA6-4B90-4E8F-8262-8D80E188C77F}">
   <dimension ref="B3:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed on betsy computer
changed on betsy computer
</commit_message>
<xml_diff>
--- a/excel test with ploot.xlsx
+++ b/excel test with ploot.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbalc\OneDrive\Documents\AAA git\Pre-FDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbalc\OneDrive\Documents\GitHub Repositories Testing\Pre-FDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20004" windowHeight="8316" xr2:uid="{C3F4FD49-A990-41F6-B6BD-74CE04A0DA08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20010" windowHeight="8310" xr2:uid="{C3F4FD49-A990-41F6-B6BD-74CE04A0DA08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$3:$B$20</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$3:$C$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3:$B$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$3:$C$20</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -219,43 +217,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,58 +622,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2677,8 +2675,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8469630" y="1203960"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="8221980" y="1249680"/>
+              <a:ext cx="4419600" cy="2857500"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3010,157 +3008,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB833DA6-4B90-4E8F-8262-8D80E188C77F}">
   <dimension ref="B3:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>17</v>
       </c>
       <c r="C19" s="1">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>